<commit_message>
Documento Aceptacion Firmado por director
</commit_message>
<xml_diff>
--- a/Documento_Aceptacion.xlsx
+++ b/Documento_Aceptacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepus Perez Flores\Documents\DAW2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/memovazquez/Desktop/DawEquipo/DAW2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BE6E53-7B98-4705-9BA1-EBEC575B57D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930F5AC1-77A1-1546-B828-4C8A39647283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{EB1B7718-A0ED-4F41-AC1A-BF63AE854246}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20400" xr2:uid="{EB1B7718-A0ED-4F41-AC1A-BF63AE854246}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,20 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Alumno</t>
   </si>
   <si>
-    <t>Iniciar Examen</t>
-  </si>
-  <si>
-    <t>Terminar examen</t>
-  </si>
-  <si>
-    <t>Reanudar Examen</t>
-  </si>
-  <si>
     <t>Administrador</t>
   </si>
   <si>
@@ -59,39 +50,6 @@
     <t>Crear Pregunta</t>
   </si>
   <si>
-    <t>Crear Texto Pregunta</t>
-  </si>
-  <si>
-    <t>Seleccionar Recurso de Pregunta</t>
-  </si>
-  <si>
-    <t>Seleccionar Materia de Pregunta</t>
-  </si>
-  <si>
-    <t>Crear Reactivo</t>
-  </si>
-  <si>
-    <t>Crear Texto Reactivo</t>
-  </si>
-  <si>
-    <t>Editar Examen</t>
-  </si>
-  <si>
-    <t>Guardar Edicion Examen</t>
-  </si>
-  <si>
-    <t>Eliminar Examen</t>
-  </si>
-  <si>
-    <t>Iniciar Sesion</t>
-  </si>
-  <si>
-    <t>Cerrar Sesion</t>
-  </si>
-  <si>
-    <t>Recuperar contraseña</t>
-  </si>
-  <si>
     <t>Nombre Requisito funcional</t>
   </si>
   <si>
@@ -107,9 +65,6 @@
     <t>Juan Manuel Amador Perez Flores</t>
   </si>
   <si>
-    <t xml:space="preserve">Guillermo </t>
-  </si>
-  <si>
     <t>Fernando Ruiz</t>
   </si>
   <si>
@@ -128,14 +83,62 @@
     <t>Herramienta digital para el proceso de selección</t>
   </si>
   <si>
-    <t>Seleccionar Recurso de Reactivo</t>
+    <t>Visualizacion de alumnos registrados</t>
+  </si>
+  <si>
+    <t>Cambio de contraseña de alumnos</t>
+  </si>
+  <si>
+    <t>Visualizacion de alumnos conectados</t>
+  </si>
+  <si>
+    <t>Alta Alumnos</t>
+  </si>
+  <si>
+    <t>Visualizar Usuario</t>
+  </si>
+  <si>
+    <t>Dar de Alta usuarios</t>
+  </si>
+  <si>
+    <t>Editar Usuario</t>
+  </si>
+  <si>
+    <t>Eliminar Usuario</t>
+  </si>
+  <si>
+    <t>Agregar Materia</t>
+  </si>
+  <si>
+    <t>Raziel Baruc Hernandez</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aceptado </t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Director. Eduardo Ortega</t>
+  </si>
+  <si>
+    <t>Aumentar tamaño de letra</t>
+  </si>
+  <si>
+    <t>Notas de advertencia</t>
+  </si>
+  <si>
+    <t>Guillermo Vazquez Cervantes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +163,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -221,16 +239,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -248,7 +269,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -544,265 +565,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEDA331-AEC1-4486-8EE3-74CD69988B60}">
-  <dimension ref="C2:G25"/>
+  <dimension ref="C2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C7" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="7">
+        <v>43966</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="7">
+        <v>43966</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C11" s="2" t="s">
+      <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G21" s="8">
+        <v>43966</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>